<commit_message>
Added Team Progress in index.html
</commit_message>
<xml_diff>
--- a/Teams Progress/AIDS-Teams-withLeaders.xlsx
+++ b/Teams Progress/AIDS-Teams-withLeaders.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Professional Documents\Training-Teaching\bv-raju\training-materials\Teams Progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB74B35-DE02-4243-B3F5-4A96E9241591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB852E0-D1C7-48D3-AE41-76E6945E129A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Team Progress" sheetId="16" r:id="rId1"/>
+    <sheet name="Team Progress" sheetId="17" r:id="rId1"/>
     <sheet name="Team_1" sheetId="1" r:id="rId2"/>
     <sheet name="Team_2" sheetId="2" r:id="rId3"/>
     <sheet name="Team_3" sheetId="3" r:id="rId4"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="307">
   <si>
     <t>Student ID</t>
   </si>
@@ -937,13 +937,25 @@
     <t>Simple Webapp demo</t>
   </si>
   <si>
-    <t>Team 1</t>
-  </si>
-  <si>
-    <t>Team 2</t>
-  </si>
-  <si>
-    <t>Good Job practicing, need to demo going forward. Presented by ????</t>
+    <t>Team 7</t>
+  </si>
+  <si>
+    <t>Update on Annotation Based Bean Configuration</t>
+  </si>
+  <si>
+    <t>Team 10</t>
+  </si>
+  <si>
+    <t>Reserved for tomorrow</t>
+  </si>
+  <si>
+    <t>Facing running issues which will co-ordinate with team 7</t>
+  </si>
+  <si>
+    <t>Done - Awaiting demo</t>
+  </si>
+  <si>
+    <t>Good Job - For names check the Team  sheet</t>
   </si>
 </sst>
 </file>
@@ -972,7 +984,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -987,6 +999,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1018,7 +1036,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1026,6 +1044,12 @@
     <xf numFmtId="14" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1339,26 +1363,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B501C087-B371-45CB-9584-F9546CB23DB3}">
-  <dimension ref="A2:D10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB2CF979-CDA0-4226-93A7-A51EEC2AA166}">
+  <dimension ref="A2:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
     <col min="3" max="3" width="41.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="84.21875" customWidth="1"/>
+    <col min="4" max="4" width="91.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="7" t="s">
         <v>287</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -1373,7 +1397,7 @@
         <v>45839</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>291</v>
@@ -1385,51 +1409,53 @@
         <v>45839</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>293</v>
+        <v>302</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>306</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>45839</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>306</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>45839</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>302</v>
-      </c>
+      <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>45839</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>297</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1437,13 +1463,13 @@
         <v>45839</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>297</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1451,10 +1477,10 @@
         <v>45840</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="D9" s="2"/>
     </row>
@@ -1463,12 +1489,28 @@
         <v>45840</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="D10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
+        <v>45840</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>305</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1477,105 +1519,119 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" s="10">
+        <v>45839</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>162</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="8" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" s="8"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>166</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="8" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5" s="8"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="8" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6" s="8"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="8" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7" s="8"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>174</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>176</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="8" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10" s="8"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>180</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>181</v>
       </c>
+      <c r="C11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1584,105 +1640,119 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" s="10">
+        <v>45839</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>182</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" s="8"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>184</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>186</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4" s="8"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>188</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>190</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>192</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>194</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>196</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>198</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>200</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>201</v>
       </c>
+      <c r="C11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2374,105 +2444,119 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" s="10">
+        <v>45839</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4" s="8"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="9" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5" s="8"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="9" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6" s="8"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="9" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7" s="8"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="9" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="9" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9" s="8"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>61</v>
       </c>
+      <c r="C11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
SPring boot intro commit
</commit_message>
<xml_diff>
--- a/Teams Progress/AIDS-Teams-withLeaders.xlsx
+++ b/Teams Progress/AIDS-Teams-withLeaders.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Professional Documents\Training-Teaching\bv-raju\training-materials\Teams Progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB852E0-D1C7-48D3-AE41-76E6945E129A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D5227C-FB72-4546-AECB-C32D332235DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="6" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team Progress" sheetId="17" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="312">
   <si>
     <t>Student ID</t>
   </si>
@@ -946,16 +946,31 @@
     <t>Team 10</t>
   </si>
   <si>
-    <t>Reserved for tomorrow</t>
-  </si>
-  <si>
     <t>Facing running issues which will co-ordinate with team 7</t>
   </si>
   <si>
-    <t>Done - Awaiting demo</t>
-  </si>
-  <si>
     <t>Good Job - For names check the Team  sheet</t>
+  </si>
+  <si>
+    <t>Team 1</t>
+  </si>
+  <si>
+    <t>Team 2</t>
+  </si>
+  <si>
+    <t>Fantastic job demoing webapp without spring framework</t>
+  </si>
+  <si>
+    <t>Reserved for 04/07</t>
+  </si>
+  <si>
+    <t>2 Team members demoed Java based configuration</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cv                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                    </t>
+  </si>
+  <si>
+    <t>t7</t>
   </si>
 </sst>
 </file>
@@ -984,7 +999,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1008,8 +1023,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1032,11 +1059,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1048,8 +1086,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1364,7 +1407,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB2CF979-CDA0-4226-93A7-A51EEC2AA166}">
-  <dimension ref="A2:D11"/>
+  <dimension ref="A2:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
@@ -1396,7 +1439,7 @@
       <c r="A3" s="6">
         <v>45839</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>290</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -1408,14 +1451,14 @@
       <c r="A4" s="6">
         <v>45839</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>302</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>291</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1429,14 +1472,14 @@
         <v>296</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>45839</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>293</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -1455,7 +1498,7 @@
         <v>297</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>303</v>
+        <v>309</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1469,14 +1512,14 @@
         <v>297</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>45840</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="15" t="s">
         <v>292</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -1495,7 +1538,7 @@
         <v>299</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1509,7 +1552,23 @@
         <v>299</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B12" s="14" t="s">
         <v>305</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B13" s="14" t="s">
+        <v>306</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -1521,7 +1580,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -1539,7 +1598,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10">
+      <c r="C1" s="9">
         <v>45839</v>
       </c>
     </row>
@@ -1660,7 +1719,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10">
+      <c r="C1" s="9">
         <v>45839</v>
       </c>
     </row>
@@ -2189,9 +2248,11 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2199,7 +2260,7 @@
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2207,15 +2268,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>282</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>284</v>
       </c>
@@ -2464,7 +2528,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10">
+      <c r="C1" s="9">
         <v>45839</v>
       </c>
     </row>
@@ -2499,7 +2563,7 @@
       <c r="A5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C5" s="8"/>
@@ -2508,7 +2572,7 @@
       <c r="A6" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C6" s="8"/>
@@ -2517,7 +2581,7 @@
       <c r="A7" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C7" s="8"/>
@@ -2526,7 +2590,7 @@
       <c r="A8" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="2" t="s">
         <v>55</v>
       </c>
       <c r="C8" s="2"/>
@@ -2535,7 +2599,7 @@
       <c r="A9" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="2" t="s">
         <v>57</v>
       </c>
       <c r="C9" s="8"/>
@@ -2556,7 +2620,7 @@
       <c r="B11" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C11" s="2"/>
+      <c r="C11" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2565,35 +2629,40 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D1" s="9">
+        <v>45840</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D2" s="11"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>64</v>
       </c>
@@ -2601,7 +2670,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>66</v>
       </c>
@@ -2609,7 +2678,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>68</v>
       </c>
@@ -2617,15 +2686,16 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D6" s="11"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>72</v>
       </c>
@@ -2633,7 +2703,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>74</v>
       </c>
@@ -2641,7 +2711,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>76</v>
       </c>
@@ -2649,7 +2719,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>78</v>
       </c>
@@ -2657,7 +2727,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>80</v>
       </c>
@@ -2886,27 +2956,31 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D1" s="10">
+        <v>45839</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>122</v>
       </c>
@@ -2914,15 +2988,16 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>124</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D3" s="12"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>126</v>
       </c>
@@ -2930,47 +3005,52 @@
         <v>127</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>128</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D5" s="11"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>130</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D6" s="11"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>132</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D7" s="11"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>134</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D8" s="11"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>136</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D9" s="11"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>138</v>
       </c>
@@ -2978,13 +3058,14 @@
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>140</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>141</v>
       </c>
+      <c r="D11" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added intro to JDBC and tracked team progress until spring rest controller
</commit_message>
<xml_diff>
--- a/Teams Progress/AIDS-Teams-withLeaders.xlsx
+++ b/Teams Progress/AIDS-Teams-withLeaders.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Professional Documents\Training-Teaching\bv-raju\training-materials\Teams Progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE5E4D11-2EFB-4F68-A0CC-AEEEE8EA323A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1EEF89-AD31-4990-9256-87374F2616F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team_1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="308">
   <si>
     <t>Student ID</t>
   </si>
@@ -909,6 +909,54 @@
   </si>
   <si>
     <t>Spring Boot Web Project</t>
+  </si>
+  <si>
+    <t>Spring Boot Rest Controller</t>
+  </si>
+  <si>
+    <t>absent</t>
+  </si>
+  <si>
+    <t>Returned back and need to catch up with the stuff</t>
+  </si>
+  <si>
+    <t>Absent</t>
+  </si>
+  <si>
+    <t>Return from internship</t>
+  </si>
+  <si>
+    <t>Tomorrow</t>
+  </si>
+  <si>
+    <t>Pending to practice</t>
+  </si>
+  <si>
+    <t>Pending to Practice</t>
+  </si>
+  <si>
+    <t>Back to college and needs refreshment</t>
+  </si>
+  <si>
+    <t>Pending for tomorrow</t>
+  </si>
+  <si>
+    <t>Reserved for tomrrow</t>
+  </si>
+  <si>
+    <t>Demoed together with Team 7</t>
+  </si>
+  <si>
+    <t>Ready with demo</t>
+  </si>
+  <si>
+    <t>End of the day Demo</t>
+  </si>
+  <si>
+    <t>reserved for tomorrow</t>
+  </si>
+  <si>
+    <t>tomorrow</t>
   </si>
 </sst>
 </file>
@@ -935,7 +983,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -965,8 +1013,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -989,11 +1043,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1004,6 +1069,10 @@
     <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1318,10 +1387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:H1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1330,7 +1399,7 @@
     <col min="2" max="2" width="26.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="78" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="78" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1355,85 +1424,118 @@
       <c r="H1" s="7" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="8" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>21</v>
+      </c>
+      <c r="I11" t="s">
+        <v>293</v>
       </c>
     </row>
   </sheetData>
@@ -1443,10 +1545,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1456,7 +1558,7 @@
     <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="78" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="78" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1481,8 +1583,11 @@
       <c r="H1" s="7" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="8" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>182</v>
       </c>
@@ -1491,7 +1596,7 @@
       </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>184</v>
       </c>
@@ -1500,7 +1605,7 @@
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>186</v>
       </c>
@@ -1508,8 +1613,9 @@
         <v>187</v>
       </c>
       <c r="C4" s="4"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>188</v>
       </c>
@@ -1518,7 +1624,7 @@
       </c>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>190</v>
       </c>
@@ -1527,7 +1633,7 @@
       </c>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>192</v>
       </c>
@@ -1536,16 +1642,16 @@
       </c>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="9" t="s">
         <v>195</v>
       </c>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>196</v>
       </c>
@@ -1553,8 +1659,9 @@
         <v>197</v>
       </c>
       <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>198</v>
       </c>
@@ -1562,8 +1669,9 @@
         <v>199</v>
       </c>
       <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>200</v>
       </c>
@@ -1579,10 +1687,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1591,7 +1699,7 @@
     <col min="2" max="2" width="24.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="78" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="78" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1616,8 +1724,11 @@
       <c r="H1" s="7" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="8" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>202</v>
       </c>
@@ -1625,23 +1736,27 @@
         <v>203</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="9" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>206</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>208</v>
       </c>
@@ -1649,7 +1764,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>210</v>
       </c>
@@ -1657,15 +1772,18 @@
         <v>211</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>212</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>214</v>
       </c>
@@ -1673,7 +1791,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>216</v>
       </c>
@@ -1681,20 +1799,24 @@
         <v>217</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>218</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>220</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>221</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -1704,10 +1826,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:H1"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1716,7 +1838,7 @@
     <col min="2" max="2" width="32.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="78" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="78" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1741,16 +1863,22 @@
       <c r="H1" s="7" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="8" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>222</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>224</v>
       </c>
@@ -1758,15 +1886,15 @@
         <v>225</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="9" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>228</v>
       </c>
@@ -1774,7 +1902,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>230</v>
       </c>
@@ -1782,23 +1910,29 @@
         <v>231</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>232</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>234</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>236</v>
       </c>
@@ -1806,7 +1940,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>238</v>
       </c>
@@ -1814,12 +1948,15 @@
         <v>239</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>240</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>241</v>
+      </c>
+      <c r="I11" t="s">
+        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -1829,10 +1966,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:H1"/>
+      <selection activeCell="I3" sqref="I3:I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1841,7 +1978,7 @@
     <col min="2" max="2" width="32.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="78" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="78" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1866,8 +2003,11 @@
       <c r="H1" s="7" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="8" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>242</v>
       </c>
@@ -1875,15 +2015,16 @@
         <v>243</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>244</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>246</v>
       </c>
@@ -1891,7 +2032,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>248</v>
       </c>
@@ -1899,7 +2040,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>250</v>
       </c>
@@ -1907,15 +2048,16 @@
         <v>251</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>252</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>254</v>
       </c>
@@ -1923,7 +2065,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>256</v>
       </c>
@@ -1931,7 +2073,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>258</v>
       </c>
@@ -1939,13 +2081,14 @@
         <v>259</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="9" t="s">
         <v>261</v>
       </c>
+      <c r="I11" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1954,10 +2097,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:H1"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1966,7 +2109,7 @@
     <col min="2" max="2" width="28.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="78" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="78" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1991,16 +2134,19 @@
       <c r="H1" s="7" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="8" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="9" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>264</v>
       </c>
@@ -2008,7 +2154,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>266</v>
       </c>
@@ -2016,15 +2162,18 @@
         <v>267</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>268</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>270</v>
       </c>
@@ -2032,7 +2181,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>272</v>
       </c>
@@ -2040,7 +2189,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>274</v>
       </c>
@@ -2048,7 +2197,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>276</v>
       </c>
@@ -2056,15 +2205,18 @@
         <v>277</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>278</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>280</v>
       </c>
@@ -2079,10 +2231,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:H1"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2091,7 +2243,7 @@
     <col min="2" max="2" width="27.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="78" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="78" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2116,85 +2268,123 @@
       <c r="H1" s="7" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="8" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>41</v>
+      </c>
+      <c r="I11" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I12" t="s">
+        <v>295</v>
       </c>
     </row>
   </sheetData>
@@ -2204,10 +2394,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2217,7 +2407,7 @@
     <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="78" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="78" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2242,8 +2432,11 @@
       <c r="H1" s="7" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="8" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>42</v>
       </c>
@@ -2252,7 +2445,7 @@
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>44</v>
       </c>
@@ -2260,8 +2453,9 @@
         <v>45</v>
       </c>
       <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>46</v>
       </c>
@@ -2270,16 +2464,17 @@
       </c>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="9" t="s">
         <v>49</v>
       </c>
       <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>50</v>
       </c>
@@ -2287,8 +2482,9 @@
         <v>51</v>
       </c>
       <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>52</v>
       </c>
@@ -2296,8 +2492,9 @@
         <v>53</v>
       </c>
       <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>54</v>
       </c>
@@ -2305,8 +2502,9 @@
         <v>55</v>
       </c>
       <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>56</v>
       </c>
@@ -2314,8 +2512,9 @@
         <v>57</v>
       </c>
       <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>58</v>
       </c>
@@ -2324,7 +2523,7 @@
       </c>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>60</v>
       </c>
@@ -2332,6 +2531,9 @@
         <v>61</v>
       </c>
       <c r="D11" s="4"/>
+      <c r="I11" t="s">
+        <v>305</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2340,10 +2542,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E6"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2353,7 +2555,7 @@
     <col min="4" max="4" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="78" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="78" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2378,8 +2580,11 @@
       <c r="H1" s="7" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="8" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>62</v>
       </c>
@@ -2388,23 +2593,29 @@
       </c>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="9" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>68</v>
       </c>
@@ -2412,7 +2623,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>70</v>
       </c>
@@ -2421,7 +2632,7 @@
       </c>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>72</v>
       </c>
@@ -2429,7 +2640,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>74</v>
       </c>
@@ -2437,7 +2648,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>76</v>
       </c>
@@ -2445,15 +2656,18 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>80</v>
       </c>
@@ -2468,10 +2682,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:H1"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2480,7 +2694,7 @@
     <col min="2" max="2" width="23.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="78" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="78" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2505,16 +2719,20 @@
       <c r="H1" s="7" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="8" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="9" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>84</v>
       </c>
@@ -2522,7 +2740,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>86</v>
       </c>
@@ -2530,15 +2748,16 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>90</v>
       </c>
@@ -2546,7 +2765,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>92</v>
       </c>
@@ -2554,7 +2773,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>94</v>
       </c>
@@ -2562,7 +2781,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>96</v>
       </c>
@@ -2570,7 +2789,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>98</v>
       </c>
@@ -2578,7 +2797,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>100</v>
       </c>
@@ -2593,10 +2812,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:H1"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2605,7 +2824,7 @@
     <col min="2" max="2" width="31.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="78" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="78" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2630,8 +2849,11 @@
       <c r="H1" s="7" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="8" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>102</v>
       </c>
@@ -2639,7 +2861,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>104</v>
       </c>
@@ -2647,7 +2869,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>106</v>
       </c>
@@ -2655,7 +2877,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>108</v>
       </c>
@@ -2663,23 +2885,25 @@
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>110</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="9" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>114</v>
       </c>
@@ -2687,7 +2911,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>116</v>
       </c>
@@ -2695,7 +2919,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>118</v>
       </c>
@@ -2703,12 +2927,15 @@
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>120</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>121</v>
+      </c>
+      <c r="I11" t="s">
+        <v>296</v>
       </c>
     </row>
   </sheetData>
@@ -2718,10 +2945,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2731,7 +2958,7 @@
     <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="78" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="78" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2756,8 +2983,11 @@
       <c r="H1" s="7" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="8" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>122</v>
       </c>
@@ -2765,7 +2995,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>124</v>
       </c>
@@ -2774,7 +3004,7 @@
       </c>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>126</v>
       </c>
@@ -2782,7 +3012,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>128</v>
       </c>
@@ -2791,7 +3021,7 @@
       </c>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>130</v>
       </c>
@@ -2800,7 +3030,7 @@
       </c>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>132</v>
       </c>
@@ -2809,7 +3039,7 @@
       </c>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>134</v>
       </c>
@@ -2818,7 +3048,7 @@
       </c>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>136</v>
       </c>
@@ -2827,7 +3057,7 @@
       </c>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>138</v>
       </c>
@@ -2835,7 +3065,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>140</v>
       </c>
@@ -2844,12 +3074,15 @@
       </c>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="9" t="s">
         <v>283</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>304</v>
       </c>
     </row>
   </sheetData>
@@ -2859,10 +3092,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:H1"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2871,7 +3104,7 @@
     <col min="2" max="2" width="33.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="78" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="78" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2896,93 +3129,129 @@
       <c r="H1" s="7" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="8" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>144</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>146</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>148</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>150</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="9" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>154</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>156</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>158</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>160</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I11" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>284</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>285</v>
+      </c>
+      <c r="I12" t="s">
+        <v>295</v>
       </c>
     </row>
   </sheetData>
@@ -2992,10 +3261,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3005,7 +3274,7 @@
     <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="78" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="78" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3030,8 +3299,11 @@
       <c r="H1" s="7" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="8" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>162</v>
       </c>
@@ -3040,16 +3312,17 @@
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="9" t="s">
         <v>165</v>
       </c>
       <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>166</v>
       </c>
@@ -3058,7 +3331,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>168</v>
       </c>
@@ -3067,7 +3340,7 @@
       </c>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>170</v>
       </c>
@@ -3076,7 +3349,7 @@
       </c>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>172</v>
       </c>
@@ -3085,7 +3358,7 @@
       </c>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>174</v>
       </c>
@@ -3094,7 +3367,7 @@
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>176</v>
       </c>
@@ -3103,16 +3376,17 @@
       </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>179</v>
       </c>
       <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>180</v>
       </c>

</xml_diff>

<commit_message>
Added Spring JDBC contd.... section
</commit_message>
<xml_diff>
--- a/Teams Progress/AIDS-Teams-withLeaders.xlsx
+++ b/Teams Progress/AIDS-Teams-withLeaders.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Professional Documents\Training-Teaching\bv-raju\training-materials\Teams Progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1EEF89-AD31-4990-9256-87374F2616F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADAC084B-14DA-4DF2-95A8-D9CB90F954E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team_1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="306">
   <si>
     <t>Student ID</t>
   </si>
@@ -933,12 +933,6 @@
   </si>
   <si>
     <t>Pending to Practice</t>
-  </si>
-  <si>
-    <t>Back to college and needs refreshment</t>
-  </si>
-  <si>
-    <t>Pending for tomorrow</t>
   </si>
   <si>
     <t>Reserved for tomrrow</t>
@@ -1480,7 +1474,7 @@
         <v>11</v>
       </c>
       <c r="I6" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -1689,7 +1683,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
@@ -1816,7 +1810,7 @@
         <v>221</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
   </sheetData>
@@ -1875,7 +1869,7 @@
         <v>223</v>
       </c>
       <c r="I2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -1918,7 +1912,7 @@
         <v>233</v>
       </c>
       <c r="I7" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -1929,7 +1923,7 @@
         <v>235</v>
       </c>
       <c r="I8" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -1956,7 +1950,7 @@
         <v>241</v>
       </c>
       <c r="I11" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>
@@ -2099,8 +2093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2153,6 +2147,7 @@
       <c r="B3" s="2" t="s">
         <v>265</v>
       </c>
+      <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -2169,9 +2164,7 @@
       <c r="B5" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="I5" t="s">
-        <v>301</v>
-      </c>
+      <c r="I5" s="5"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
@@ -2212,9 +2205,7 @@
       <c r="B10" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="I10" t="s">
-        <v>300</v>
-      </c>
+      <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
@@ -2532,7 +2523,7 @@
       </c>
       <c r="D11" s="4"/>
       <c r="I11" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -2601,7 +2592,7 @@
         <v>65</v>
       </c>
       <c r="I3" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -2612,7 +2603,7 @@
         <v>67</v>
       </c>
       <c r="I4" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -2664,7 +2655,7 @@
         <v>79</v>
       </c>
       <c r="I10" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -3082,7 +3073,7 @@
         <v>283</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added reference project links for JDBC section
</commit_message>
<xml_diff>
--- a/Teams Progress/AIDS-Teams-withLeaders.xlsx
+++ b/Teams Progress/AIDS-Teams-withLeaders.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Professional Documents\Training-Teaching\bv-raju\training-materials\Teams Progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADAC084B-14DA-4DF2-95A8-D9CB90F954E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76BD231-7B3E-42F1-B703-4CF9675CE7F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team_1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="315">
   <si>
     <t>Student ID</t>
   </si>
@@ -951,6 +951,33 @@
   </si>
   <si>
     <t>tomorrow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Practice and for demo skipped the class </t>
+  </si>
+  <si>
+    <t>For demo skipped the class when asked</t>
+  </si>
+  <si>
+    <t>Demoed Spring JDBC curd operations</t>
+  </si>
+  <si>
+    <t>Good with spring jdbc demo</t>
+  </si>
+  <si>
+    <t>A section Lab</t>
+  </si>
+  <si>
+    <t>Saturday Morning</t>
+  </si>
+  <si>
+    <t>B section Lab</t>
+  </si>
+  <si>
+    <t>Wednesday afternoon</t>
+  </si>
+  <si>
+    <t>Good Spring JDBC, Rest Controller end to end demo</t>
   </si>
 </sst>
 </file>
@@ -977,7 +1004,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1010,6 +1037,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1052,7 +1085,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1067,6 +1100,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1381,10 +1415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1393,7 +1427,7 @@
     <col min="2" max="2" width="26.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="78" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="78" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1422,7 +1456,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1433,7 +1467,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1444,7 +1478,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1455,18 +1489,21 @@
         <v>293</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="10" t="s">
         <v>9</v>
       </c>
       <c r="I5" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J5" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1477,7 +1514,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -1488,7 +1525,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -1499,7 +1536,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -1510,7 +1547,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -1521,7 +1558,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -1530,6 +1567,22 @@
       </c>
       <c r="I11" t="s">
         <v>293</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>310</v>
+      </c>
+      <c r="B16" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>312</v>
+      </c>
+      <c r="B17" t="s">
+        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -1820,10 +1873,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1832,7 +1885,7 @@
     <col min="2" max="2" width="32.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="78" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="78" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1861,7 +1914,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>222</v>
       </c>
@@ -1872,7 +1925,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>224</v>
       </c>
@@ -1880,7 +1933,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>226</v>
       </c>
@@ -1888,7 +1941,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>228</v>
       </c>
@@ -1896,7 +1949,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>230</v>
       </c>
@@ -1904,7 +1957,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>232</v>
       </c>
@@ -1915,7 +1968,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>234</v>
       </c>
@@ -1925,8 +1978,11 @@
       <c r="I8" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J8" s="5" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>236</v>
       </c>
@@ -1934,7 +1990,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>238</v>
       </c>
@@ -1942,7 +1998,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>240</v>
       </c>
@@ -2093,8 +2149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2385,10 +2441,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2398,7 +2454,7 @@
     <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="78" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="78" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2427,7 +2483,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>42</v>
       </c>
@@ -2436,7 +2492,7 @@
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>44</v>
       </c>
@@ -2446,7 +2502,7 @@
       <c r="C3" s="2"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>46</v>
       </c>
@@ -2455,7 +2511,7 @@
       </c>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>48</v>
       </c>
@@ -2465,7 +2521,7 @@
       <c r="D5" s="4"/>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>50</v>
       </c>
@@ -2475,7 +2531,7 @@
       <c r="D6" s="4"/>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>52</v>
       </c>
@@ -2485,17 +2541,20 @@
       <c r="D7" s="4"/>
       <c r="I7" s="5"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="10" t="s">
         <v>55</v>
       </c>
       <c r="D8" s="2"/>
       <c r="I8" s="5"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J8" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>56</v>
       </c>
@@ -2505,7 +2564,7 @@
       <c r="D9" s="4"/>
       <c r="I9" s="5"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>58</v>
       </c>
@@ -2514,7 +2573,7 @@
       </c>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>60</v>
       </c>
@@ -2936,10 +2995,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2949,7 +3008,7 @@
     <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="78" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="78" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2978,7 +3037,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>122</v>
       </c>
@@ -2986,7 +3045,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>124</v>
       </c>
@@ -2995,7 +3054,7 @@
       </c>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>126</v>
       </c>
@@ -3003,7 +3062,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>128</v>
       </c>
@@ -3012,7 +3071,7 @@
       </c>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>130</v>
       </c>
@@ -3021,7 +3080,7 @@
       </c>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>132</v>
       </c>
@@ -3030,7 +3089,7 @@
       </c>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>134</v>
       </c>
@@ -3039,7 +3098,7 @@
       </c>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>136</v>
       </c>
@@ -3048,7 +3107,7 @@
       </c>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>138</v>
       </c>
@@ -3056,7 +3115,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>140</v>
       </c>
@@ -3065,7 +3124,7 @@
       </c>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>282</v>
       </c>
@@ -3074,6 +3133,9 @@
       </c>
       <c r="I12" s="5" t="s">
         <v>302</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -3086,7 +3148,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3252,10 +3314,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3265,7 +3327,7 @@
     <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="78" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="78" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3294,7 +3356,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>162</v>
       </c>
@@ -3303,7 +3365,7 @@
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>164</v>
       </c>
@@ -3313,7 +3375,7 @@
       <c r="E3" s="4"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>166</v>
       </c>
@@ -3322,7 +3384,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>168</v>
       </c>
@@ -3330,8 +3392,11 @@
         <v>169</v>
       </c>
       <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J5" s="5" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>170</v>
       </c>
@@ -3340,7 +3405,7 @@
       </c>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>172</v>
       </c>
@@ -3349,7 +3414,7 @@
       </c>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>174</v>
       </c>
@@ -3358,7 +3423,7 @@
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>176</v>
       </c>
@@ -3367,7 +3432,7 @@
       </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>178</v>
       </c>
@@ -3377,7 +3442,7 @@
       <c r="E10" s="4"/>
       <c r="I10" s="5"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>180</v>
       </c>

</xml_diff>

<commit_message>
Added SOLID and design patterns
</commit_message>
<xml_diff>
--- a/Teams Progress/AIDS-Teams-withLeaders.xlsx
+++ b/Teams Progress/AIDS-Teams-withLeaders.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Professional Documents\Training-Teaching\bv-raju\training-materials\Teams Progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{928C2233-E8BC-4EA1-A844-C754930473B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45217170-8546-499F-BC92-7D6BE8EC0468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1129,7 +1129,7 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFFC000"/>
+          <fgColor rgb="FF92D050"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -1448,7 +1448,7 @@
   <dimension ref="A1:K143"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="155" zoomScaleNormal="155" workbookViewId="0">
-      <selection activeCell="I57" sqref="I57"/>
+      <selection activeCell="K120" sqref="K6:K120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1548,7 +1548,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1591,7 +1591,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
@@ -1813,7 +1813,7 @@
       </c>
       <c r="E24" s="4"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>48</v>
       </c>
@@ -1917,7 +1917,7 @@
       </c>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>64</v>
       </c>
@@ -2026,7 +2026,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>82</v>
       </c>
@@ -2060,7 +2060,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>88</v>
       </c>
@@ -2084,7 +2084,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>92</v>
       </c>
@@ -2196,7 +2196,7 @@
       </c>
       <c r="J56" s="5"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>112</v>
       </c>
@@ -2372,7 +2372,7 @@
       </c>
       <c r="G71" s="5"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>282</v>
       </c>
@@ -2456,7 +2456,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>152</v>
       </c>
@@ -2552,7 +2552,7 @@
       </c>
       <c r="D84" s="2"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>164</v>
       </c>
@@ -2577,7 +2577,7 @@
       </c>
       <c r="F86" s="2"/>
     </row>
-    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>168</v>
       </c>
@@ -2689,7 +2689,7 @@
       </c>
       <c r="D95" s="2"/>
     </row>
-    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>186</v>
       </c>
@@ -2754,7 +2754,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="101" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>196</v>
       </c>
@@ -2804,7 +2804,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>204</v>
       </c>
@@ -2928,7 +2928,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="115" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>224</v>
       </c>
@@ -2940,7 +2940,7 @@
       </c>
       <c r="K115" s="5"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>226</v>
       </c>
@@ -2987,7 +2987,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="120" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>234</v>
       </c>
@@ -3141,7 +3141,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>260</v>
       </c>
@@ -3153,7 +3153,7 @@
       </c>
       <c r="J133" s="5"/>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>262</v>
       </c>
@@ -3268,7 +3268,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:K143" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="1">
+    <filterColumn colId="10">
       <colorFilter dxfId="0"/>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Added to do app design
</commit_message>
<xml_diff>
--- a/Teams Progress/AIDS-Teams-withLeaders.xlsx
+++ b/Teams Progress/AIDS-Teams-withLeaders.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Professional Documents\Training-Teaching\bv-raju\training-materials\Teams Progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45217170-8546-499F-BC92-7D6BE8EC0468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B478DC-E216-4538-B7C9-DF1ACF75E91A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1024,7 +1024,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1063,6 +1063,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1105,7 +1111,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1121,20 +1127,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1444,11 +1442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:K143"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="155" zoomScaleNormal="155" workbookViewId="0">
-      <selection activeCell="K120" sqref="K6:K120"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1492,7 +1489,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1506,7 +1503,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1520,7 +1517,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1534,7 +1531,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1563,7 +1560,7 @@
       </c>
       <c r="K6" s="5"/>
     </row>
-    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -1577,7 +1574,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -1591,7 +1588,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -1605,7 +1602,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -1619,7 +1616,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -1633,7 +1630,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -1647,7 +1644,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -1661,7 +1658,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
@@ -1675,7 +1672,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
@@ -1689,7 +1686,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
@@ -1703,7 +1700,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
@@ -1717,7 +1714,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>34</v>
       </c>
@@ -1731,7 +1728,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>36</v>
       </c>
@@ -1745,7 +1742,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>38</v>
       </c>
@@ -1759,7 +1756,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>40</v>
       </c>
@@ -1773,7 +1770,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>42</v>
       </c>
@@ -1788,7 +1785,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>44</v>
       </c>
@@ -1801,7 +1798,7 @@
       <c r="D23" s="2"/>
       <c r="J23" s="5"/>
     </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>46</v>
       </c>
@@ -1813,7 +1810,7 @@
       </c>
       <c r="E24" s="4"/>
     </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>48</v>
       </c>
@@ -1826,7 +1823,7 @@
       <c r="E25" s="4"/>
       <c r="J25" s="5"/>
     </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>50</v>
       </c>
@@ -1839,7 +1836,7 @@
       <c r="E26" s="4"/>
       <c r="J26" s="5"/>
     </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>52</v>
       </c>
@@ -1852,7 +1849,7 @@
       <c r="E27" s="4"/>
       <c r="J27" s="5"/>
     </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>54</v>
       </c>
@@ -1865,7 +1862,7 @@
       <c r="E28" s="2"/>
       <c r="J28" s="5"/>
     </row>
-    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>56</v>
       </c>
@@ -1878,7 +1875,7 @@
       <c r="E29" s="4"/>
       <c r="J29" s="5"/>
     </row>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>58</v>
       </c>
@@ -1890,7 +1887,7 @@
       </c>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>60</v>
       </c>
@@ -1905,7 +1902,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>62</v>
       </c>
@@ -1917,7 +1914,7 @@
       </c>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>64</v>
       </c>
@@ -1931,7 +1928,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>66</v>
       </c>
@@ -1945,7 +1942,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>68</v>
       </c>
@@ -1956,7 +1953,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>70</v>
       </c>
@@ -1968,7 +1965,7 @@
       </c>
       <c r="F36" s="5"/>
     </row>
-    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>72</v>
       </c>
@@ -1979,7 +1976,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>74</v>
       </c>
@@ -1990,7 +1987,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>76</v>
       </c>
@@ -2001,7 +1998,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>78</v>
       </c>
@@ -2015,7 +2012,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>80</v>
       </c>
@@ -2026,7 +2023,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>82</v>
       </c>
@@ -2038,7 +2035,7 @@
       </c>
       <c r="J42" s="5"/>
     </row>
-    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>84</v>
       </c>
@@ -2049,7 +2046,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>86</v>
       </c>
@@ -2064,7 +2061,7 @@
       <c r="A45" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="4" t="s">
         <v>89</v>
       </c>
       <c r="C45" t="s">
@@ -2073,7 +2070,7 @@
       <c r="J45" s="5"/>
       <c r="K45" s="5"/>
     </row>
-    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>90</v>
       </c>
@@ -2096,7 +2093,7 @@
       </c>
       <c r="K47" s="5"/>
     </row>
-    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>94</v>
       </c>
@@ -2107,7 +2104,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>96</v>
       </c>
@@ -2118,7 +2115,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>98</v>
       </c>
@@ -2129,7 +2126,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>100</v>
       </c>
@@ -2140,7 +2137,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>102</v>
       </c>
@@ -2151,7 +2148,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>104</v>
       </c>
@@ -2162,7 +2159,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>106</v>
       </c>
@@ -2173,7 +2170,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>108</v>
       </c>
@@ -2184,7 +2181,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>110</v>
       </c>
@@ -2196,7 +2193,7 @@
       </c>
       <c r="J56" s="5"/>
     </row>
-    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>112</v>
       </c>
@@ -2208,7 +2205,7 @@
       </c>
       <c r="J57" s="5"/>
     </row>
-    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>114</v>
       </c>
@@ -2219,7 +2216,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>116</v>
       </c>
@@ -2230,7 +2227,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>118</v>
       </c>
@@ -2241,7 +2238,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>120</v>
       </c>
@@ -2255,7 +2252,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>122</v>
       </c>
@@ -2266,7 +2263,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>124</v>
       </c>
@@ -2278,7 +2275,7 @@
       </c>
       <c r="E63" s="6"/>
     </row>
-    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>126</v>
       </c>
@@ -2289,7 +2286,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>128</v>
       </c>
@@ -2301,7 +2298,7 @@
       </c>
       <c r="G65" s="5"/>
     </row>
-    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>130</v>
       </c>
@@ -2313,7 +2310,7 @@
       </c>
       <c r="G66" s="5"/>
     </row>
-    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>132</v>
       </c>
@@ -2325,11 +2322,11 @@
       </c>
       <c r="G67" s="5"/>
     </row>
-    <row r="68" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B68" s="11" t="s">
         <v>135</v>
       </c>
       <c r="C68" t="s">
@@ -2337,7 +2334,7 @@
       </c>
       <c r="G68" s="5"/>
     </row>
-    <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>136</v>
       </c>
@@ -2349,7 +2346,7 @@
       </c>
       <c r="G69" s="5"/>
     </row>
-    <row r="70" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>138</v>
       </c>
@@ -2360,7 +2357,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>140</v>
       </c>
@@ -2372,7 +2369,7 @@
       </c>
       <c r="G71" s="5"/>
     </row>
-    <row r="72" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>282</v>
       </c>
@@ -2386,7 +2383,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>142</v>
       </c>
@@ -2400,7 +2397,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>144</v>
       </c>
@@ -2414,7 +2411,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="75" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>146</v>
       </c>
@@ -2428,7 +2425,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>148</v>
       </c>
@@ -2442,7 +2439,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>150</v>
       </c>
@@ -2456,7 +2453,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>152</v>
       </c>
@@ -2470,7 +2467,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>154</v>
       </c>
@@ -2484,7 +2481,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>156</v>
       </c>
@@ -2498,7 +2495,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="81" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>158</v>
       </c>
@@ -2512,7 +2509,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>160</v>
       </c>
@@ -2526,7 +2523,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>284</v>
       </c>
@@ -2540,7 +2537,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>162</v>
       </c>
@@ -2552,7 +2549,7 @@
       </c>
       <c r="D84" s="2"/>
     </row>
-    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>164</v>
       </c>
@@ -2565,7 +2562,7 @@
       <c r="F85" s="4"/>
       <c r="J85" s="5"/>
     </row>
-    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>166</v>
       </c>
@@ -2581,7 +2578,7 @@
       <c r="A87" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="B87" s="4" t="s">
         <v>169</v>
       </c>
       <c r="C87" t="s">
@@ -2592,7 +2589,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>170</v>
       </c>
@@ -2604,7 +2601,7 @@
       </c>
       <c r="F88" s="4"/>
     </row>
-    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>172</v>
       </c>
@@ -2616,7 +2613,7 @@
       </c>
       <c r="F89" s="4"/>
     </row>
-    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>174</v>
       </c>
@@ -2628,7 +2625,7 @@
       </c>
       <c r="F90" s="2"/>
     </row>
-    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>176</v>
       </c>
@@ -2640,11 +2637,11 @@
       </c>
       <c r="F91" s="2"/>
     </row>
-    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B92" s="3" t="s">
+      <c r="B92" s="4" t="s">
         <v>179</v>
       </c>
       <c r="C92" t="s">
@@ -2653,7 +2650,7 @@
       <c r="F92" s="4"/>
       <c r="J92" s="5"/>
     </row>
-    <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>180</v>
       </c>
@@ -2665,7 +2662,7 @@
       </c>
       <c r="F93" s="2"/>
     </row>
-    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>182</v>
       </c>
@@ -2677,7 +2674,7 @@
       </c>
       <c r="D94" s="4"/>
     </row>
-    <row r="95" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>184</v>
       </c>
@@ -2703,7 +2700,7 @@
       <c r="J96" s="5"/>
       <c r="K96" s="5"/>
     </row>
-    <row r="97" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>188</v>
       </c>
@@ -2715,7 +2712,7 @@
       </c>
       <c r="D97" s="2"/>
     </row>
-    <row r="98" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>190</v>
       </c>
@@ -2727,7 +2724,7 @@
       </c>
       <c r="D98" s="2"/>
     </row>
-    <row r="99" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>192</v>
       </c>
@@ -2743,7 +2740,7 @@
       <c r="A100" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="B100" s="9" t="s">
+      <c r="B100" s="4" t="s">
         <v>195</v>
       </c>
       <c r="C100" t="s">
@@ -2758,7 +2755,7 @@
       <c r="A101" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="B101" s="2" t="s">
+      <c r="B101" s="11" t="s">
         <v>197</v>
       </c>
       <c r="C101" t="s">
@@ -2768,7 +2765,7 @@
       <c r="J101" s="5"/>
       <c r="K101" s="5"/>
     </row>
-    <row r="102" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>198</v>
       </c>
@@ -2781,7 +2778,7 @@
       <c r="D102" s="2"/>
       <c r="J102" s="5"/>
     </row>
-    <row r="103" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>200</v>
       </c>
@@ -2793,7 +2790,7 @@
       </c>
       <c r="D103" s="2"/>
     </row>
-    <row r="104" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>202</v>
       </c>
@@ -2804,7 +2801,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="105" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>204</v>
       </c>
@@ -2818,7 +2815,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="106" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>206</v>
       </c>
@@ -2830,7 +2827,7 @@
       </c>
       <c r="J106" s="5"/>
     </row>
-    <row r="107" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>208</v>
       </c>
@@ -2841,7 +2838,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="108" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>210</v>
       </c>
@@ -2852,7 +2849,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="109" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>212</v>
       </c>
@@ -2866,7 +2863,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="110" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>214</v>
       </c>
@@ -2877,7 +2874,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="111" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>216</v>
       </c>
@@ -2888,7 +2885,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="112" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>218</v>
       </c>
@@ -2900,7 +2897,7 @@
       </c>
       <c r="J112" s="5"/>
     </row>
-    <row r="113" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>220</v>
       </c>
@@ -2914,7 +2911,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="114" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>222</v>
       </c>
@@ -2940,7 +2937,7 @@
       </c>
       <c r="K115" s="5"/>
     </row>
-    <row r="116" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>226</v>
       </c>
@@ -2951,7 +2948,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="117" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>228</v>
       </c>
@@ -2962,7 +2959,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="118" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>230</v>
       </c>
@@ -2973,7 +2970,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="119" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>232</v>
       </c>
@@ -3004,7 +3001,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="121" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>236</v>
       </c>
@@ -3015,7 +3012,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="122" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>238</v>
       </c>
@@ -3026,7 +3023,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="123" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>240</v>
       </c>
@@ -3040,7 +3037,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="124" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>242</v>
       </c>
@@ -3051,7 +3048,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="125" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>244</v>
       </c>
@@ -3063,7 +3060,7 @@
       </c>
       <c r="J125" s="5"/>
     </row>
-    <row r="126" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>246</v>
       </c>
@@ -3074,7 +3071,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="127" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>248</v>
       </c>
@@ -3085,7 +3082,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="128" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>250</v>
       </c>
@@ -3096,7 +3093,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="129" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>252</v>
       </c>
@@ -3108,7 +3105,7 @@
       </c>
       <c r="J129" s="5"/>
     </row>
-    <row r="130" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>254</v>
       </c>
@@ -3119,7 +3116,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="131" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>256</v>
       </c>
@@ -3130,7 +3127,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="132" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>258</v>
       </c>
@@ -3141,7 +3138,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="133" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>260</v>
       </c>
@@ -3153,7 +3150,7 @@
       </c>
       <c r="J133" s="5"/>
     </row>
-    <row r="134" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>262</v>
       </c>
@@ -3164,7 +3161,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="135" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>264</v>
       </c>
@@ -3176,7 +3173,7 @@
       </c>
       <c r="J135" s="5"/>
     </row>
-    <row r="136" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>266</v>
       </c>
@@ -3187,7 +3184,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="137" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>268</v>
       </c>
@@ -3199,7 +3196,7 @@
       </c>
       <c r="J137" s="5"/>
     </row>
-    <row r="138" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>270</v>
       </c>
@@ -3210,7 +3207,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="139" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>272</v>
       </c>
@@ -3221,7 +3218,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="140" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>274</v>
       </c>
@@ -3232,7 +3229,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="141" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>276</v>
       </c>
@@ -3243,7 +3240,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="142" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
         <v>278</v>
       </c>
@@ -3255,7 +3252,7 @@
       </c>
       <c r="J142" s="5"/>
     </row>
-    <row r="143" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
         <v>280</v>
       </c>
@@ -3267,11 +3264,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K143" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="10">
-      <colorFilter dxfId="0"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:K143" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>